<commit_message>
Mock test batch updated
Mock test batch updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Information/CollegeDoors/MockTest/MockTest-Batch.xlsx
+++ b/Offline/BusinessManagement/Information/CollegeDoors/MockTest/MockTest-Batch.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Information\CollegeDoors\MockTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3388D635-4BDA-4872-9940-EB62D777A7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD61F4D8-3184-4AF8-BFD8-A9395068A317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Batch" sheetId="6" r:id="rId1"/>
+    <sheet name="Dec-2023" sheetId="6" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Student Name</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Gurdian Name</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Student's Phone No</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>Moore Avenue</t>
   </si>
   <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
@@ -106,6 +100,21 @@
   </si>
   <si>
     <t>Remarks In Comments</t>
+  </si>
+  <si>
+    <t>Room-No</t>
+  </si>
+  <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>Avishek Adhikary</t>
+  </si>
+  <si>
+    <t>Invigilator</t>
+  </si>
+  <si>
+    <t>Enrollment Status</t>
   </si>
 </sst>
 </file>
@@ -198,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -236,19 +245,18 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P122"/>
+  <dimension ref="A1:S122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -541,1265 +549,1642 @@
     <col min="2" max="2" width="9.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" customWidth="1"/>
-    <col min="16" max="16" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" customWidth="1"/>
+    <col min="8" max="8" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" customWidth="1"/>
+    <col min="18" max="18" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="31.2" customHeight="1">
+    <row r="1" spans="1:19" ht="31.2" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" s="20" customFormat="1" ht="14.4" customHeight="1">
+    </row>
+    <row r="2" spans="1:19" ht="14.4" customHeight="1">
       <c r="A2" s="15">
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="16">
         <v>45262</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="15"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="18">
+        <v>9830610602</v>
+      </c>
+      <c r="N2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="18">
-        <v>9830610602</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="17" t="s">
+      <c r="O2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="20"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:19">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:19">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="8"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="8"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:19">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:19">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:19">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:19">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="8"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="8"/>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="1:13">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="8"/>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="8"/>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="1:13">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="8"/>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="8"/>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="1:13">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="8"/>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="8"/>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" spans="1:13">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="8"/>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="8"/>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="8"/>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="8"/>
+    </row>
+    <row r="25" spans="1:13">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="8"/>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="8"/>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="8"/>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="8"/>
+    </row>
+    <row r="27" spans="1:13">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="8"/>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="8"/>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="8"/>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="8"/>
+    </row>
+    <row r="29" spans="1:13">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="8"/>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="8"/>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="8"/>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="8"/>
+    </row>
+    <row r="31" spans="1:13">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="8"/>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="8"/>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="8"/>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="8"/>
+    </row>
+    <row r="33" spans="1:13">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="8"/>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="8"/>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="8"/>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="8"/>
+    </row>
+    <row r="35" spans="1:13">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="8"/>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="8"/>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="8"/>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="8"/>
+    </row>
+    <row r="37" spans="1:13">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="8"/>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="8"/>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="8"/>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="8"/>
+    </row>
+    <row r="39" spans="1:13">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="8"/>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="8"/>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="8"/>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="8"/>
+    </row>
+    <row r="41" spans="1:13">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="8"/>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="8"/>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="8"/>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="8"/>
+    </row>
+    <row r="43" spans="1:13">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="8"/>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="8"/>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="8"/>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="8"/>
+    </row>
+    <row r="45" spans="1:13">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="8"/>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="8"/>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="10"/>
-      <c r="H46"/>
-      <c r="J46" s="2"/>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="10"/>
+      <c r="K46"/>
+      <c r="M46" s="2"/>
+    </row>
+    <row r="47" spans="1:13">
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="10"/>
-      <c r="H47"/>
-      <c r="J47" s="2"/>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="10"/>
+      <c r="K47"/>
+      <c r="M47" s="2"/>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="10"/>
-      <c r="H48"/>
-      <c r="J48" s="2"/>
-    </row>
-    <row r="49" spans="1:10">
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="10"/>
+      <c r="K48"/>
+      <c r="M48" s="2"/>
+    </row>
+    <row r="49" spans="1:13">
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
-      <c r="G49" s="10"/>
-      <c r="H49"/>
-      <c r="J49" s="2"/>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="10"/>
+      <c r="K49"/>
+      <c r="M49" s="2"/>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
-      <c r="G50" s="10"/>
-      <c r="H50"/>
-      <c r="J50" s="2"/>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="10"/>
+      <c r="K50"/>
+      <c r="M50" s="2"/>
+    </row>
+    <row r="51" spans="1:13">
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
-      <c r="G51" s="10"/>
-      <c r="H51"/>
-      <c r="J51" s="2"/>
-    </row>
-    <row r="52" spans="1:10">
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="10"/>
+      <c r="K51"/>
+      <c r="M51" s="2"/>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
-      <c r="G52" s="10"/>
-      <c r="H52"/>
-      <c r="J52" s="2"/>
-    </row>
-    <row r="53" spans="1:10">
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="10"/>
+      <c r="K52"/>
+      <c r="M52" s="2"/>
+    </row>
+    <row r="53" spans="1:13">
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
-      <c r="G53" s="10"/>
-      <c r="H53"/>
-      <c r="J53" s="2"/>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="10"/>
+      <c r="K53"/>
+      <c r="M53" s="2"/>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
-      <c r="G54" s="10"/>
-      <c r="H54"/>
-      <c r="J54" s="2"/>
-    </row>
-    <row r="55" spans="1:10">
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="10"/>
+      <c r="K54"/>
+      <c r="M54" s="2"/>
+    </row>
+    <row r="55" spans="1:13">
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
-      <c r="G55" s="10"/>
-      <c r="H55"/>
-      <c r="J55" s="2"/>
-    </row>
-    <row r="56" spans="1:10">
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="10"/>
+      <c r="K55"/>
+      <c r="M55" s="2"/>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
-      <c r="G56" s="10"/>
-      <c r="H56"/>
-      <c r="J56" s="2"/>
-    </row>
-    <row r="57" spans="1:10">
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="10"/>
+      <c r="K56"/>
+      <c r="M56" s="2"/>
+    </row>
+    <row r="57" spans="1:13">
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
-      <c r="G57" s="10"/>
-      <c r="H57"/>
-      <c r="J57" s="2"/>
-    </row>
-    <row r="58" spans="1:10">
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="10"/>
+      <c r="K57"/>
+      <c r="M57" s="2"/>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
-      <c r="G58" s="10"/>
-      <c r="H58"/>
-      <c r="J58" s="2"/>
-    </row>
-    <row r="59" spans="1:10">
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="10"/>
+      <c r="K58"/>
+      <c r="M58" s="2"/>
+    </row>
+    <row r="59" spans="1:13">
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
-      <c r="G59" s="10"/>
-      <c r="H59"/>
-      <c r="J59" s="2"/>
-    </row>
-    <row r="60" spans="1:10">
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="10"/>
+      <c r="K59"/>
+      <c r="M59" s="2"/>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
-      <c r="G60" s="10"/>
-      <c r="H60"/>
-      <c r="J60" s="2"/>
-    </row>
-    <row r="61" spans="1:10">
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="10"/>
+      <c r="K60"/>
+      <c r="M60" s="2"/>
+    </row>
+    <row r="61" spans="1:13">
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
-      <c r="G61" s="10"/>
-      <c r="H61"/>
-      <c r="J61" s="2"/>
-    </row>
-    <row r="62" spans="1:10">
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="10"/>
+      <c r="K61"/>
+      <c r="M61" s="2"/>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
-      <c r="G62" s="10"/>
-      <c r="H62"/>
-      <c r="J62" s="2"/>
-    </row>
-    <row r="63" spans="1:10">
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="10"/>
+      <c r="K62"/>
+      <c r="M62" s="2"/>
+    </row>
+    <row r="63" spans="1:13">
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
-      <c r="G63" s="10"/>
-      <c r="H63"/>
-      <c r="J63" s="2"/>
-    </row>
-    <row r="64" spans="1:10">
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="10"/>
+      <c r="K63"/>
+      <c r="M63" s="2"/>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
-      <c r="G64" s="10"/>
-      <c r="H64"/>
-      <c r="J64" s="2"/>
-    </row>
-    <row r="65" spans="1:10">
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="10"/>
+      <c r="K64"/>
+      <c r="M64" s="2"/>
+    </row>
+    <row r="65" spans="1:13">
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
-      <c r="G65" s="10"/>
-      <c r="H65"/>
-      <c r="J65" s="2"/>
-    </row>
-    <row r="66" spans="1:10">
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="10"/>
+      <c r="K65"/>
+      <c r="M65" s="2"/>
+    </row>
+    <row r="66" spans="1:13">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
-      <c r="G66" s="10"/>
-      <c r="H66"/>
-      <c r="J66" s="2"/>
-    </row>
-    <row r="67" spans="1:10">
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="10"/>
+      <c r="K66"/>
+      <c r="M66" s="2"/>
+    </row>
+    <row r="67" spans="1:13">
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
-      <c r="G67" s="10"/>
-      <c r="H67"/>
-      <c r="J67" s="2"/>
-    </row>
-    <row r="68" spans="1:10">
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="10"/>
+      <c r="K67"/>
+      <c r="M67" s="2"/>
+    </row>
+    <row r="68" spans="1:13">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
-      <c r="G68" s="10"/>
-      <c r="H68"/>
-      <c r="J68" s="2"/>
-    </row>
-    <row r="69" spans="1:10">
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="10"/>
+      <c r="K68"/>
+      <c r="M68" s="2"/>
+    </row>
+    <row r="69" spans="1:13">
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
-      <c r="G69" s="10"/>
-      <c r="H69"/>
-      <c r="J69" s="2"/>
-    </row>
-    <row r="70" spans="1:10">
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="10"/>
+      <c r="K69"/>
+      <c r="M69" s="2"/>
+    </row>
+    <row r="70" spans="1:13">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
-      <c r="G70" s="10"/>
-      <c r="H70"/>
-      <c r="J70" s="2"/>
-    </row>
-    <row r="71" spans="1:10">
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="10"/>
+      <c r="K70"/>
+      <c r="M70" s="2"/>
+    </row>
+    <row r="71" spans="1:13">
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
-      <c r="G71" s="10"/>
-      <c r="H71"/>
-      <c r="J71" s="2"/>
-    </row>
-    <row r="72" spans="1:10">
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="10"/>
+      <c r="K71"/>
+      <c r="M71" s="2"/>
+    </row>
+    <row r="72" spans="1:13">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
-      <c r="G72" s="10"/>
-      <c r="H72"/>
-      <c r="J72" s="2"/>
-    </row>
-    <row r="73" spans="1:10">
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="10"/>
+      <c r="K72"/>
+      <c r="M72" s="2"/>
+    </row>
+    <row r="73" spans="1:13">
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
-      <c r="G73" s="10"/>
-      <c r="H73"/>
-      <c r="J73" s="2"/>
-    </row>
-    <row r="74" spans="1:10">
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="10"/>
+      <c r="K73"/>
+      <c r="M73" s="2"/>
+    </row>
+    <row r="74" spans="1:13">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
-      <c r="G74" s="10"/>
-      <c r="H74"/>
-      <c r="J74" s="2"/>
-    </row>
-    <row r="75" spans="1:10">
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="10"/>
+      <c r="K74"/>
+      <c r="M74" s="2"/>
+    </row>
+    <row r="75" spans="1:13">
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
-      <c r="G75" s="10"/>
-      <c r="H75"/>
-      <c r="J75" s="2"/>
-    </row>
-    <row r="76" spans="1:10">
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="10"/>
+      <c r="K75"/>
+      <c r="M75" s="2"/>
+    </row>
+    <row r="76" spans="1:13">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
-      <c r="G76" s="10"/>
-      <c r="H76"/>
-      <c r="J76" s="2"/>
-    </row>
-    <row r="77" spans="1:10">
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="10"/>
+      <c r="K76"/>
+      <c r="M76" s="2"/>
+    </row>
+    <row r="77" spans="1:13">
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
-      <c r="G77" s="10"/>
-      <c r="H77"/>
-      <c r="J77" s="2"/>
-    </row>
-    <row r="78" spans="1:10">
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="10"/>
+      <c r="K77"/>
+      <c r="M77" s="2"/>
+    </row>
+    <row r="78" spans="1:13">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
-      <c r="G78" s="10"/>
-      <c r="H78"/>
-      <c r="J78" s="2"/>
-    </row>
-    <row r="79" spans="1:10">
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="10"/>
+      <c r="K78"/>
+      <c r="M78" s="2"/>
+    </row>
+    <row r="79" spans="1:13">
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
-      <c r="G79" s="11"/>
-      <c r="H79"/>
-      <c r="J79" s="2"/>
-    </row>
-    <row r="80" spans="1:10">
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="11"/>
+      <c r="K79"/>
+      <c r="M79" s="2"/>
+    </row>
+    <row r="80" spans="1:13">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
-      <c r="G80" s="11"/>
-      <c r="H80"/>
-      <c r="J80" s="2"/>
-    </row>
-    <row r="81" spans="1:10">
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="11"/>
+      <c r="K80"/>
+      <c r="M80" s="2"/>
+    </row>
+    <row r="81" spans="1:13">
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
-      <c r="G81" s="11"/>
-      <c r="H81"/>
-      <c r="J81" s="2"/>
-    </row>
-    <row r="82" spans="1:10">
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="11"/>
+      <c r="K81"/>
+      <c r="M81" s="2"/>
+    </row>
+    <row r="82" spans="1:13">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
-      <c r="G82" s="11"/>
-      <c r="H82"/>
-      <c r="J82" s="2"/>
-    </row>
-    <row r="83" spans="1:10">
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="11"/>
+      <c r="K82"/>
+      <c r="M82" s="2"/>
+    </row>
+    <row r="83" spans="1:13">
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
-      <c r="G83" s="10"/>
-      <c r="H83"/>
-      <c r="J83" s="2"/>
-    </row>
-    <row r="84" spans="1:10">
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="10"/>
+      <c r="K83"/>
+      <c r="M83" s="2"/>
+    </row>
+    <row r="84" spans="1:13">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
-      <c r="G84" s="10"/>
-      <c r="H84"/>
-      <c r="J84" s="2"/>
-    </row>
-    <row r="85" spans="1:10">
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="10"/>
+      <c r="K84"/>
+      <c r="M84" s="2"/>
+    </row>
+    <row r="85" spans="1:13">
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
-      <c r="G85" s="11"/>
-      <c r="H85"/>
-      <c r="J85" s="2"/>
-    </row>
-    <row r="86" spans="1:10">
+      <c r="G85" s="4"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="11"/>
+      <c r="K85"/>
+      <c r="M85" s="2"/>
+    </row>
+    <row r="86" spans="1:13">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
-      <c r="G86" s="11"/>
-      <c r="H86"/>
-      <c r="J86" s="2"/>
-    </row>
-    <row r="87" spans="1:10">
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="11"/>
+      <c r="K86"/>
+      <c r="M86" s="2"/>
+    </row>
+    <row r="87" spans="1:13">
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
-      <c r="G87" s="10"/>
-      <c r="H87"/>
-      <c r="J87" s="2"/>
-    </row>
-    <row r="88" spans="1:10">
+      <c r="G87" s="4"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="10"/>
+      <c r="K87"/>
+      <c r="M87" s="2"/>
+    </row>
+    <row r="88" spans="1:13">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
-      <c r="G88" s="10"/>
-      <c r="H88"/>
-      <c r="J88" s="2"/>
-    </row>
-    <row r="89" spans="1:10">
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="10"/>
+      <c r="K88"/>
+      <c r="M88" s="2"/>
+    </row>
+    <row r="89" spans="1:13">
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
-      <c r="G89" s="10"/>
-      <c r="H89"/>
-      <c r="J89" s="2"/>
-    </row>
-    <row r="90" spans="1:10">
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="10"/>
+      <c r="K89"/>
+      <c r="M89" s="2"/>
+    </row>
+    <row r="90" spans="1:13">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
-      <c r="G90" s="10"/>
-      <c r="H90"/>
-      <c r="J90" s="2"/>
-    </row>
-    <row r="91" spans="1:10">
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="10"/>
+      <c r="K90"/>
+      <c r="M90" s="2"/>
+    </row>
+    <row r="91" spans="1:13">
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
-      <c r="G91" s="10"/>
-      <c r="H91"/>
-      <c r="J91" s="2"/>
-    </row>
-    <row r="92" spans="1:10">
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="10"/>
+      <c r="K91"/>
+      <c r="M91" s="2"/>
+    </row>
+    <row r="92" spans="1:13">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
-      <c r="G92" s="10"/>
-      <c r="H92"/>
-      <c r="J92" s="2"/>
-    </row>
-    <row r="93" spans="1:10">
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="10"/>
+      <c r="K92"/>
+      <c r="M92" s="2"/>
+    </row>
+    <row r="93" spans="1:13">
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
-      <c r="G93" s="10"/>
-      <c r="H93"/>
-      <c r="J93" s="2"/>
-    </row>
-    <row r="94" spans="1:10">
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="10"/>
+      <c r="K93"/>
+      <c r="M93" s="2"/>
+    </row>
+    <row r="94" spans="1:13">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
-      <c r="G94" s="10"/>
-      <c r="H94"/>
-      <c r="J94" s="2"/>
-    </row>
-    <row r="95" spans="1:10">
+      <c r="G94" s="4"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
+      <c r="J94" s="10"/>
+      <c r="K94"/>
+      <c r="M94" s="2"/>
+    </row>
+    <row r="95" spans="1:13">
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
-      <c r="G95" s="10"/>
-      <c r="H95"/>
-      <c r="J95" s="2"/>
-    </row>
-    <row r="96" spans="1:10">
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
+      <c r="J95" s="10"/>
+      <c r="K95"/>
+      <c r="M95" s="2"/>
+    </row>
+    <row r="96" spans="1:13">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
-      <c r="G96" s="10"/>
-      <c r="H96"/>
-      <c r="J96" s="2"/>
-    </row>
-    <row r="97" spans="1:10">
+      <c r="G96" s="4"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
+      <c r="J96" s="10"/>
+      <c r="K96"/>
+      <c r="M96" s="2"/>
+    </row>
+    <row r="97" spans="1:13">
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
-      <c r="G97" s="10"/>
-      <c r="H97"/>
-      <c r="J97" s="2"/>
-    </row>
-    <row r="98" spans="1:10">
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="4"/>
+      <c r="J97" s="10"/>
+      <c r="K97"/>
+      <c r="M97" s="2"/>
+    </row>
+    <row r="98" spans="1:13">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
-      <c r="G98" s="10"/>
-      <c r="H98"/>
-      <c r="J98" s="2"/>
-    </row>
-    <row r="99" spans="1:10">
+      <c r="G98" s="4"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="4"/>
+      <c r="J98" s="10"/>
+      <c r="K98"/>
+      <c r="M98" s="2"/>
+    </row>
+    <row r="99" spans="1:13">
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
-      <c r="G99" s="10"/>
-      <c r="H99"/>
-      <c r="J99" s="2"/>
-    </row>
-    <row r="100" spans="1:10">
+      <c r="G99" s="4"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="4"/>
+      <c r="J99" s="10"/>
+      <c r="K99"/>
+      <c r="M99" s="2"/>
+    </row>
+    <row r="100" spans="1:13">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
       <c r="F100" s="4"/>
-      <c r="G100" s="10"/>
-      <c r="H100"/>
-      <c r="J100" s="2"/>
-    </row>
-    <row r="101" spans="1:10">
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="4"/>
+      <c r="J100" s="10"/>
+      <c r="K100"/>
+      <c r="M100" s="2"/>
+    </row>
+    <row r="101" spans="1:13">
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
-      <c r="G101" s="10"/>
-      <c r="H101"/>
-      <c r="J101" s="2"/>
-    </row>
-    <row r="102" spans="1:10">
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="4"/>
+      <c r="J101" s="10"/>
+      <c r="K101"/>
+      <c r="M101" s="2"/>
+    </row>
+    <row r="102" spans="1:13">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
-      <c r="G102" s="10"/>
-      <c r="H102"/>
-      <c r="J102" s="2"/>
-    </row>
-    <row r="103" spans="1:10">
+      <c r="G102" s="4"/>
+      <c r="H102" s="4"/>
+      <c r="I102" s="4"/>
+      <c r="J102" s="10"/>
+      <c r="K102"/>
+      <c r="M102" s="2"/>
+    </row>
+    <row r="103" spans="1:13">
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
       <c r="F103" s="4"/>
-      <c r="G103" s="10"/>
-      <c r="H103"/>
-      <c r="J103" s="2"/>
-    </row>
-    <row r="104" spans="1:10">
+      <c r="G103" s="4"/>
+      <c r="H103" s="4"/>
+      <c r="I103" s="4"/>
+      <c r="J103" s="10"/>
+      <c r="K103"/>
+      <c r="M103" s="2"/>
+    </row>
+    <row r="104" spans="1:13">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
-      <c r="G104" s="10"/>
-      <c r="H104"/>
-      <c r="J104" s="2"/>
-    </row>
-    <row r="105" spans="1:10">
+      <c r="G104" s="4"/>
+      <c r="H104" s="4"/>
+      <c r="I104" s="4"/>
+      <c r="J104" s="10"/>
+      <c r="K104"/>
+      <c r="M104" s="2"/>
+    </row>
+    <row r="105" spans="1:13">
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
-      <c r="G105" s="10"/>
-      <c r="H105"/>
-      <c r="J105" s="2"/>
-    </row>
-    <row r="106" spans="1:10">
+      <c r="G105" s="4"/>
+      <c r="H105" s="4"/>
+      <c r="I105" s="4"/>
+      <c r="J105" s="10"/>
+      <c r="K105"/>
+      <c r="M105" s="2"/>
+    </row>
+    <row r="106" spans="1:13">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
-      <c r="G106" s="10"/>
-      <c r="H106"/>
-      <c r="J106" s="2"/>
-    </row>
-    <row r="107" spans="1:10">
+      <c r="G106" s="4"/>
+      <c r="H106" s="4"/>
+      <c r="I106" s="4"/>
+      <c r="J106" s="10"/>
+      <c r="K106"/>
+      <c r="M106" s="2"/>
+    </row>
+    <row r="107" spans="1:13">
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
-      <c r="G107" s="10"/>
-      <c r="H107"/>
-      <c r="J107" s="2"/>
-    </row>
-    <row r="108" spans="1:10">
+      <c r="G107" s="4"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="4"/>
+      <c r="J107" s="10"/>
+      <c r="K107"/>
+      <c r="M107" s="2"/>
+    </row>
+    <row r="108" spans="1:13">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
-      <c r="G108" s="10"/>
-      <c r="H108"/>
-      <c r="J108" s="2"/>
-    </row>
-    <row r="109" spans="1:10">
+      <c r="G108" s="4"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="4"/>
+      <c r="J108" s="10"/>
+      <c r="K108"/>
+      <c r="M108" s="2"/>
+    </row>
+    <row r="109" spans="1:13">
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
-      <c r="G109" s="10"/>
-      <c r="H109"/>
-      <c r="J109" s="2"/>
-    </row>
-    <row r="110" spans="1:10">
+      <c r="G109" s="4"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="4"/>
+      <c r="J109" s="10"/>
+      <c r="K109"/>
+      <c r="M109" s="2"/>
+    </row>
+    <row r="110" spans="1:13">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
-      <c r="G110" s="10"/>
-      <c r="H110"/>
-      <c r="J110" s="2"/>
-    </row>
-    <row r="111" spans="1:10">
+      <c r="G110" s="4"/>
+      <c r="H110" s="4"/>
+      <c r="I110" s="4"/>
+      <c r="J110" s="10"/>
+      <c r="K110"/>
+      <c r="M110" s="2"/>
+    </row>
+    <row r="111" spans="1:13">
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
-      <c r="G111" s="10"/>
-      <c r="H111"/>
-      <c r="J111" s="2"/>
-    </row>
-    <row r="112" spans="1:10">
+      <c r="G111" s="4"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="4"/>
+      <c r="J111" s="10"/>
+      <c r="K111"/>
+      <c r="M111" s="2"/>
+    </row>
+    <row r="112" spans="1:13">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
-      <c r="G112" s="10"/>
-      <c r="H112"/>
-      <c r="J112" s="2"/>
-    </row>
-    <row r="113" spans="1:10">
+      <c r="G112" s="4"/>
+      <c r="H112" s="4"/>
+      <c r="I112" s="4"/>
+      <c r="J112" s="10"/>
+      <c r="K112"/>
+      <c r="M112" s="2"/>
+    </row>
+    <row r="113" spans="1:13">
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
-      <c r="G113" s="10"/>
-      <c r="H113"/>
-      <c r="J113" s="2"/>
-    </row>
-    <row r="114" spans="1:10">
+      <c r="G113" s="4"/>
+      <c r="H113" s="4"/>
+      <c r="I113" s="4"/>
+      <c r="J113" s="10"/>
+      <c r="K113"/>
+      <c r="M113" s="2"/>
+    </row>
+    <row r="114" spans="1:13">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
-      <c r="G114" s="10"/>
-      <c r="H114"/>
-      <c r="J114" s="2"/>
-    </row>
-    <row r="115" spans="1:10">
+      <c r="G114" s="4"/>
+      <c r="H114" s="4"/>
+      <c r="I114" s="4"/>
+      <c r="J114" s="10"/>
+      <c r="K114"/>
+      <c r="M114" s="2"/>
+    </row>
+    <row r="115" spans="1:13">
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
-      <c r="G115" s="10"/>
-      <c r="H115"/>
-      <c r="J115" s="2"/>
-    </row>
-    <row r="116" spans="1:10">
+      <c r="G115" s="4"/>
+      <c r="H115" s="4"/>
+      <c r="I115" s="4"/>
+      <c r="J115" s="10"/>
+      <c r="K115"/>
+      <c r="M115" s="2"/>
+    </row>
+    <row r="116" spans="1:13">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
-      <c r="G116" s="10"/>
-      <c r="H116"/>
-      <c r="J116" s="2"/>
-    </row>
-    <row r="117" spans="1:10">
+      <c r="G116" s="4"/>
+      <c r="H116" s="4"/>
+      <c r="I116" s="4"/>
+      <c r="J116" s="10"/>
+      <c r="K116"/>
+      <c r="M116" s="2"/>
+    </row>
+    <row r="117" spans="1:13">
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
-      <c r="G117" s="10"/>
-      <c r="H117"/>
-      <c r="J117" s="2"/>
-    </row>
-    <row r="118" spans="1:10">
+      <c r="G117" s="4"/>
+      <c r="H117" s="4"/>
+      <c r="I117" s="4"/>
+      <c r="J117" s="10"/>
+      <c r="K117"/>
+      <c r="M117" s="2"/>
+    </row>
+    <row r="118" spans="1:13">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
-      <c r="G118" s="10"/>
-      <c r="H118"/>
-      <c r="J118" s="2"/>
-    </row>
-    <row r="119" spans="1:10">
+      <c r="G118" s="4"/>
+      <c r="H118" s="4"/>
+      <c r="I118" s="4"/>
+      <c r="J118" s="10"/>
+      <c r="K118"/>
+      <c r="M118" s="2"/>
+    </row>
+    <row r="119" spans="1:13">
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
-      <c r="G119" s="10"/>
-      <c r="H119"/>
-      <c r="J119" s="2"/>
-    </row>
-    <row r="120" spans="1:10">
+      <c r="G119" s="4"/>
+      <c r="H119" s="4"/>
+      <c r="I119" s="4"/>
+      <c r="J119" s="10"/>
+      <c r="K119"/>
+      <c r="M119" s="2"/>
+    </row>
+    <row r="120" spans="1:13">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
-      <c r="G120" s="10"/>
-      <c r="H120"/>
-      <c r="J120" s="2"/>
-    </row>
-    <row r="121" spans="1:10">
+      <c r="G120" s="4"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="4"/>
+      <c r="J120" s="10"/>
+      <c r="K120"/>
+      <c r="M120" s="2"/>
+    </row>
+    <row r="121" spans="1:13">
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
-      <c r="G121" s="10"/>
-      <c r="H121"/>
-      <c r="J121" s="2"/>
-    </row>
-    <row r="122" spans="1:10">
+      <c r="G121" s="4"/>
+      <c r="H121" s="4"/>
+      <c r="I121" s="4"/>
+      <c r="J121" s="10"/>
+      <c r="K121"/>
+      <c r="M121" s="2"/>
+    </row>
+    <row r="122" spans="1:13">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
-      <c r="G122" s="10"/>
-      <c r="H122"/>
-      <c r="J122" s="2"/>
+      <c r="G122" s="4"/>
+      <c r="H122" s="4"/>
+      <c r="I122" s="4"/>
+      <c r="J122" s="10"/>
+      <c r="K122"/>
+      <c r="M122" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>